<commit_message>
correccion de bugs con treads
</commit_message>
<xml_diff>
--- a/Datos/Hospitales.xlsx
+++ b/Datos/Hospitales.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DanielHernandezCuero\Documents\GeneticAlgorithm\Datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{153D8D36-86EC-45A4-BD4C-DB32611E9E16}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{BE37E964-1B78-4F5A-917F-CACD26B9E6D6}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{41BA3546-1918-4C2E-9F15-FAB5A5EE3D5F}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="61">
   <si>
     <t>Clínica Nuestra Señora de los Remedios</t>
   </si>
@@ -184,6 +184,30 @@
   </si>
   <si>
     <t>Latitud</t>
+  </si>
+  <si>
+    <t>Policlinica</t>
+  </si>
+  <si>
+    <t>3.462114, -76.534489</t>
+  </si>
+  <si>
+    <t>3.378835, -76.516787</t>
+  </si>
+  <si>
+    <t>Policlinica del sur</t>
+  </si>
+  <si>
+    <t>3.447693, -76.536113</t>
+  </si>
+  <si>
+    <t>Clinica Confenalco</t>
+  </si>
+  <si>
+    <t>3.439847, -76.537950</t>
+  </si>
+  <si>
+    <t>Fundación Clínica Infantil Club Noel</t>
   </si>
 </sst>
 </file>
@@ -261,7 +285,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -285,6 +309,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -599,10 +625,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E956EA71-02A0-490C-9ABB-190AC0CD5997}">
-  <dimension ref="A1:G19"/>
+  <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B4"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27:A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -647,13 +673,13 @@
       <c r="E2" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F2" s="2" t="str">
-        <f>LEFT(E2,8)</f>
-        <v>3.463197</v>
-      </c>
-      <c r="G2" s="2" t="str">
-        <f>RIGHT(E2, LEN(E2)-10)</f>
-        <v>-76.522517</v>
+      <c r="F2" s="10" t="str">
+        <f t="shared" ref="F2:F19" si="0">SUBSTITUTE(LEFT(E2,8),".",",")</f>
+        <v>3,463197</v>
+      </c>
+      <c r="G2" s="10" t="str">
+        <f t="shared" ref="G2:G19" si="1">SUBSTITUTE(RIGHT(E2, LEN(E2)-10), ".", ",")</f>
+        <v>-76,522517</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="17.25" x14ac:dyDescent="0.25">
@@ -672,13 +698,13 @@
       <c r="E3" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="F3" s="2" t="str">
-        <f t="shared" ref="F3:F19" si="0">LEFT(E3,8)</f>
-        <v>3.454596</v>
-      </c>
-      <c r="G3" s="2" t="str">
-        <f t="shared" ref="G3:G19" si="1">RIGHT(E3, LEN(E3)-10)</f>
-        <v>-76.537206</v>
+      <c r="F3" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>3,454596</v>
+      </c>
+      <c r="G3" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>-76,537206</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="17.25" x14ac:dyDescent="0.25">
@@ -697,13 +723,13 @@
       <c r="E4" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="F4" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>3.460488</v>
-      </c>
-      <c r="G4" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>-76.530161</v>
+      <c r="F4" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>3,460488</v>
+      </c>
+      <c r="G4" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>-76,530161</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="17.25" x14ac:dyDescent="0.25">
@@ -722,13 +748,13 @@
       <c r="E5" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="F5" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>3.432143</v>
-      </c>
-      <c r="G5" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>-76.538913</v>
+      <c r="F5" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>3,432143</v>
+      </c>
+      <c r="G5" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>-76,538913</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="17.25" x14ac:dyDescent="0.25">
@@ -747,13 +773,13 @@
       <c r="E6" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F6" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>3.428015</v>
-      </c>
-      <c r="G6" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>-76.545562</v>
+      <c r="F6" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>3,428015</v>
+      </c>
+      <c r="G6" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>-76,545562</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="17.25" x14ac:dyDescent="0.25">
@@ -772,13 +798,13 @@
       <c r="E7" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="F7" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>3.372714</v>
-      </c>
-      <c r="G7" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>-76.525860</v>
+      <c r="F7" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>3,372714</v>
+      </c>
+      <c r="G7" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>-76,525860</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="17.25" x14ac:dyDescent="0.25">
@@ -797,13 +823,13 @@
       <c r="E8" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="F8" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>3.425252</v>
-      </c>
-      <c r="G8" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>-76.533494</v>
+      <c r="F8" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>3,425252</v>
+      </c>
+      <c r="G8" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>-76,533494</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="17.25" x14ac:dyDescent="0.25">
@@ -822,13 +848,13 @@
       <c r="E9" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="F9" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>3.410149</v>
-      </c>
-      <c r="G9" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>-76.539637</v>
+      <c r="F9" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>3,410149</v>
+      </c>
+      <c r="G9" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>-76,539637</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="17.25" x14ac:dyDescent="0.25">
@@ -845,13 +871,13 @@
       <c r="E10" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="F10" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>3.467292</v>
-      </c>
-      <c r="G10" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>-76.524898</v>
+      <c r="F10" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>3,467292</v>
+      </c>
+      <c r="G10" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>-76,524898</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="17.25" x14ac:dyDescent="0.25">
@@ -868,13 +894,13 @@
       <c r="E11" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="F11" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>3.470483</v>
-      </c>
-      <c r="G11" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>-76.521631</v>
+      <c r="F11" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>3,470483</v>
+      </c>
+      <c r="G11" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>-76,521631</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="17.25" x14ac:dyDescent="0.25">
@@ -891,13 +917,13 @@
       <c r="E12" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="F12" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>3.422725</v>
-      </c>
-      <c r="G12" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>-76.542499</v>
+      <c r="F12" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>3,422725</v>
+      </c>
+      <c r="G12" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>-76,542499</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -916,13 +942,13 @@
       <c r="E13" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="F13" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>3.454973</v>
-      </c>
-      <c r="G13" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>-76.527741</v>
+      <c r="F13" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>3,454973</v>
+      </c>
+      <c r="G13" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>-76,527741</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="17.25" x14ac:dyDescent="0.25">
@@ -941,13 +967,13 @@
       <c r="E14" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="F14" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>3.411540</v>
-      </c>
-      <c r="G14" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>-76.485657</v>
+      <c r="F14" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>3,411540</v>
+      </c>
+      <c r="G14" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>-76,485657</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="17.25" x14ac:dyDescent="0.25">
@@ -966,13 +992,13 @@
       <c r="E15" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="F15" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>3.430584</v>
-      </c>
-      <c r="G15" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>-76.545014</v>
+      <c r="F15" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>3,430584</v>
+      </c>
+      <c r="G15" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>-76,545014</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="17.25" x14ac:dyDescent="0.25">
@@ -991,13 +1017,13 @@
       <c r="E16" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="F16" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>3.387165</v>
-      </c>
-      <c r="G16" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>-76.558323</v>
+      <c r="F16" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>3,387165</v>
+      </c>
+      <c r="G16" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>-76,558323</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="17.25" x14ac:dyDescent="0.25">
@@ -1014,13 +1040,13 @@
       <c r="E17" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="F17" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>3.423274</v>
-      </c>
-      <c r="G17" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>-76.543761</v>
+      <c r="F17" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>3,423274</v>
+      </c>
+      <c r="G17" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>-76,543761</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="17.25" x14ac:dyDescent="0.25">
@@ -1039,13 +1065,13 @@
       <c r="E18" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="F18" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>3.409774</v>
-      </c>
-      <c r="G18" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>-76.514706</v>
+      <c r="F18" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>3,409774</v>
+      </c>
+      <c r="G18" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>-76,514706</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="17.25" x14ac:dyDescent="0.25">
@@ -1062,13 +1088,101 @@
       <c r="E19" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="F19" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>3.479143</v>
-      </c>
-      <c r="G19" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>-76.500947</v>
+      <c r="F19" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>3,479143</v>
+      </c>
+      <c r="G19" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>-76,500947</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A20" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="B20" s="8">
+        <v>-76.534488999999994</v>
+      </c>
+      <c r="C20" s="8">
+        <v>3.4621140000000001</v>
+      </c>
+      <c r="E20" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="F20" s="10" t="str">
+        <f>SUBSTITUTE(LEFT(E20,8),".",",")</f>
+        <v>3,462114</v>
+      </c>
+      <c r="G20" s="10" t="str">
+        <f>SUBSTITUTE(RIGHT(E20, LEN(E20)-10), ".", ",")</f>
+        <v>-76,534489</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A21" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="B21" s="8">
+        <v>-76.516786999999994</v>
+      </c>
+      <c r="C21" s="8">
+        <v>3.378835</v>
+      </c>
+      <c r="E21" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="F21" s="10" t="str">
+        <f>SUBSTITUTE(LEFT(E21,8),".",",")</f>
+        <v>3,378835</v>
+      </c>
+      <c r="G21" s="10" t="str">
+        <f>SUBSTITUTE(RIGHT(E21, LEN(E21)-10), ".", ",")</f>
+        <v>-76,516787</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A22" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="B22" s="8">
+        <v>-76.536113</v>
+      </c>
+      <c r="C22" s="8">
+        <v>3.4476930000000001</v>
+      </c>
+      <c r="E22" t="s">
+        <v>57</v>
+      </c>
+      <c r="F22" s="10" t="str">
+        <f>SUBSTITUTE(LEFT(E22,8),".",",")</f>
+        <v>3,447693</v>
+      </c>
+      <c r="G22" s="10" t="str">
+        <f>SUBSTITUTE(RIGHT(E22, LEN(E22)-10), ".", ",")</f>
+        <v>-76,536113</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A23" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="B23" s="8">
+        <v>-76.537949999999995</v>
+      </c>
+      <c r="C23" s="8">
+        <v>3.4398469999999999</v>
+      </c>
+      <c r="E23" t="s">
+        <v>59</v>
+      </c>
+      <c r="F23" s="10" t="str">
+        <f>SUBSTITUTE(LEFT(E23,8),".",",")</f>
+        <v>3,439847</v>
+      </c>
+      <c r="G23" s="10" t="str">
+        <f>SUBSTITUTE(RIGHT(E23, LEN(E23)-10), ".", ",")</f>
+        <v>-76,537950</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Icono y actualizacion de funciones
</commit_message>
<xml_diff>
--- a/Datos/Hospitales.xlsx
+++ b/Datos/Hospitales.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DanielHernandezCuero\Documents\GeneticAlgorithm\Datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC4855B5-0639-46DF-BFCB-703508D4AD59}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CEED387-9E4E-4115-AF3B-56ECB7201A41}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{41BA3546-1918-4C2E-9F15-FAB5A5EE3D5F}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>Clínica Nuestra Señora de los Remedios</t>
   </si>
@@ -109,20 +109,16 @@
   </si>
   <si>
     <t>Clinica Versalles Norte</t>
-  </si>
-  <si>
-    <t>TEST POINT</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.00000"/>
-    <numFmt numFmtId="172" formatCode="#,##0.000000"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -151,17 +147,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Consolas"/>
-      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -199,7 +184,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -211,12 +196,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="172" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="172" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -532,10 +511,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E956EA71-02A0-490C-9ABB-190AC0CD5997}">
-  <dimension ref="A1:F31"/>
+  <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -785,7 +764,7 @@
       <c r="C22" s="2">
         <v>3.4476930000000001</v>
       </c>
-      <c r="F22" s="7"/>
+      <c r="F22" s="5"/>
     </row>
     <row r="23" spans="1:6" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
@@ -831,26 +810,15 @@
         <v>3.4642110000000002</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="B27" s="6">
-        <v>-76.489880999999997</v>
-      </c>
-      <c r="C27" s="5">
-        <v>3.4980920000000002</v>
-      </c>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E28" s="4"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E29" s="4"/>
+      <c r="B29" s="4"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="4"/>
       <c r="B30" s="4"/>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="4"/>
-      <c r="B31" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>